<commit_message>
1. AnnotationMakerBase class introduced, all common methods are left in here, specific ones are in the child classes now 2. AnnotationMaker becomes AnnotationMakerOld for old loop drawings 3. AnnotationMakerNew is for new loop drawings: 4. Added a method for FCS annotations in AnnotationMakerNew
</commit_message>
<xml_diff>
--- a/loop_diagrams.xlsx
+++ b/loop_diagrams.xlsx
@@ -451,7 +451,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -460,8 +460,8 @@
     <col width="59.28515625" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
     <col width="31.140625" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
     <col width="84.5703125" customWidth="1" style="3" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="3" min="5" max="10"/>
-    <col width="9.140625" customWidth="1" style="3" min="11" max="16384"/>
+    <col width="9.140625" customWidth="1" style="3" min="5" max="11"/>
+    <col width="9.140625" customWidth="1" style="3" min="12" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -529,8 +529,8 @@
     <col width="40.28515625" bestFit="1" customWidth="1" style="3" min="1" max="2"/>
     <col width="31.140625" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
     <col width="84.5703125" customWidth="1" style="3" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="3" min="5" max="10"/>
-    <col width="9.140625" customWidth="1" style="3" min="11" max="16384"/>
+    <col width="9.140625" customWidth="1" style="3" min="5" max="11"/>
+    <col width="9.140625" customWidth="1" style="3" min="12" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -26133,8 +26133,8 @@
     <col width="40.28515625" bestFit="1" customWidth="1" style="3" min="1" max="2"/>
     <col width="31.140625" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
     <col width="84.5703125" customWidth="1" style="3" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="3" min="5" max="10"/>
-    <col width="9.140625" customWidth="1" style="3" min="11" max="16384"/>
+    <col width="9.140625" customWidth="1" style="3" min="5" max="11"/>
+    <col width="9.140625" customWidth="1" style="3" min="12" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>